<commit_message>
Signed-off-by: andres venegas <afvenegas10@hotmail.com>
</commit_message>
<xml_diff>
--- a/unidad de victimas/mysite/src/python_hol/static/recursos/documentos/INDEXACIÓN DIGITALIZACIÓN - FORMATO.xlsx
+++ b/unidad de victimas/mysite/src/python_hol/static/recursos/documentos/INDEXACIÓN DIGITALIZACIÓN - FORMATO.xlsx
@@ -5,9 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andres\git\web\mysite\src\python_hol\static\recursos\documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andres\git\unidad de victimas\mysite\src\python_hol\static\recursos\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="5y3fyE975+Hx+V/Dhnz+iQ6tkvSp+9yP60beYrz7ZAN4nrJlrZSkjGwfdxPUC6fGNWtnrsJze0UGM0ZJRaSmVw==" workbookSaltValue="CciSti79W4oNYi39A76PUg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855"/>
   </bookViews>
@@ -107,9 +108,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,48 +421,50 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>